<commit_message>
scale PedalPosProIncrease_Th centrally in class Config
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1031E32B-2D72-D34F-84B3-284BE3153DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916B3B08-6223-B74D-AB13-56FE8D685021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3500" windowWidth="34200" windowHeight="17180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="219">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -690,6 +690,12 @@
   </si>
   <si>
     <t>🌸 Pink</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Max throttle increase during AEB</t>
   </si>
 </sst>
 </file>
@@ -782,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -812,6 +818,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1591,469 +1598,511 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24310F59-1486-4F41-B3B7-AB25CE8F592D}">
-  <dimension ref="B2:K15"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.83203125" customWidth="1"/>
+    <col min="10" max="10" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+      <c r="K1" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="C2" s="3">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3">
+        <v>85</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
       <c r="D3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>100</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>100</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>300</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>600</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>80</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
         <v>5</v>
       </c>
-      <c r="E3" s="3">
-        <v>85</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="E12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="H12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="2" t="b">
+      <c r="J12" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="K12" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="H13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="J13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="2" t="s">
+      <c r="H14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>100</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" s="2" t="b">
+      <c r="J14" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>100</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>300</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G8" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>600</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G9" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>40</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G10" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>6</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>80</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>5</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>5</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="K14" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
params can be loaded from excel to class
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916B3B08-6223-B74D-AB13-56FE8D685021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2224EB8D-58C1-EA41-920D-F9B1B023683D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3500" windowWidth="34200" windowHeight="17180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="9580" windowWidth="34200" windowHeight="11100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -1427,166 +1427,166 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
-  <dimension ref="B2:F10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8.83203125" customWidth="1"/>
-    <col min="6" max="6" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="44.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
+    <row r="1" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="B1" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>186</v>
       </c>
-      <c r="C3">
+      <c r="B2">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>190</v>
+      </c>
       <c r="D3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5">
+        <v>-6</v>
+      </c>
+      <c r="C5" t="s">
         <v>190</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6">
+        <v>-15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="C7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B8">
+        <v>0.2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9">
+        <v>0.01</v>
+      </c>
+      <c r="C9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" t="s">
         <v>88</v>
       </c>
-      <c r="F3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>190</v>
-      </c>
-      <c r="E4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C5">
-        <v>300</v>
-      </c>
-      <c r="D5" t="s">
-        <v>203</v>
-      </c>
-      <c r="F5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C6">
-        <v>-6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E6" t="s">
-        <v>196</v>
-      </c>
-      <c r="F6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7">
-        <v>-15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>190</v>
-      </c>
-      <c r="E7" t="s">
-        <v>196</v>
-      </c>
-      <c r="F7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C8">
-        <v>-4.9000000000000004</v>
-      </c>
-      <c r="D8" t="s">
-        <v>190</v>
-      </c>
-      <c r="E8" t="s">
-        <v>196</v>
-      </c>
-      <c r="F8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C9">
-        <v>0.2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>190</v>
-      </c>
       <c r="E9" t="s">
-        <v>196</v>
-      </c>
-      <c r="F9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>202</v>
-      </c>
-      <c r="C10">
-        <v>0.01</v>
-      </c>
-      <c r="D10" t="s">
-        <v>190</v>
-      </c>
-      <c r="E10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" t="s">
         <v>206</v>
       </c>
     </row>
@@ -1601,7 +1601,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2087,7 +2087,7 @@
         <v>72</v>
       </c>
       <c r="F14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Refine logic to load params and complete the pipeline class
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2224EB8D-58C1-EA41-920D-F9B1B023683D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52A4C10-CC74-DC4C-9D6C-2B1D5EC2436D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9580" windowWidth="34200" windowHeight="11100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-520" yWindow="9860" windowWidth="34200" windowHeight="20320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -644,9 +644,6 @@
     <t>Tolerance for target deceleration</t>
   </si>
   <si>
-    <t>Time offset to account for latAccel, yawRate, and steering</t>
-  </si>
-  <si>
     <t>RE-SAMPLE</t>
   </si>
   <si>
@@ -696,6 +693,9 @@
   </si>
   <si>
     <t>Max throttle increase during AEB</t>
+  </si>
+  <si>
+    <t>samples (~3s at 0.01s rate)</t>
   </si>
 </sst>
 </file>
@@ -1135,8 +1135,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1429,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1471,7 +1472,7 @@
         <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1488,7 +1489,7 @@
         <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1499,10 +1500,10 @@
         <v>300</v>
       </c>
       <c r="C4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E4" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1575,7 +1576,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B9">
         <v>0.01</v>
@@ -1587,7 +1588,7 @@
         <v>88</v>
       </c>
       <c r="E9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1600,8 +1601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24310F59-1486-4F41-B3B7-AB25CE8F592D}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1649,7 +1650,7 @@
         <v>81</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1759,7 +1760,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>178</v>
@@ -1794,7 +1795,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>179</v>
@@ -1813,7 +1814,7 @@
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>24</v>
@@ -2834,7 +2835,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>93</v>
@@ -2846,7 +2847,7 @@
         <v>95</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
@@ -2863,7 +2864,7 @@
         <v>0.70499999999999996</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
@@ -2880,7 +2881,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
@@ -2897,7 +2898,7 @@
         <v>0.17199999999999999</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
@@ -2914,7 +2915,7 @@
         <v>0.157</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
@@ -2931,7 +2932,7 @@
         <v>0.74099999999999999</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
@@ -2948,7 +2949,7 @@
         <v>0.29399999999999998</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
@@ -2965,7 +2966,7 @@
         <v>0.76</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimize aeb event detection logic - detect_events
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52A4C10-CC74-DC4C-9D6C-2B1D5EC2436D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8EF05A-F0D2-0A41-935B-F81098573E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-520" yWindow="9860" windowWidth="34200" windowHeight="20320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="34200" windowHeight="20320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="227">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -696,6 +696,30 @@
   </si>
   <si>
     <t>samples (~3s at 0.01s rate)</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>EventDetector</t>
+  </si>
+  <si>
+    <t>START_DECEL_DELTA</t>
+  </si>
+  <si>
+    <t>threshold for large negative change (event start)</t>
+  </si>
+  <si>
+    <t>END_DECEL_DELTA</t>
+  </si>
+  <si>
+    <t># threshold for positive change (event end)</t>
+  </si>
+  <si>
+    <t>KpiExtractor</t>
+  </si>
+  <si>
+    <t>InputHandler</t>
   </si>
 </sst>
 </file>
@@ -788,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -818,7 +842,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1428,20 +1451,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="4" width="8.83203125" customWidth="1"/>
     <col min="5" max="5" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>183</v>
       </c>
@@ -1457,13 +1481,16 @@
       <c r="E1" s="10" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>0.01</v>
       </c>
       <c r="C2" t="s">
         <v>190</v>
@@ -1472,15 +1499,18 @@
         <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+      <c r="F2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>190</v>
@@ -1489,29 +1519,38 @@
         <v>88</v>
       </c>
       <c r="E3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4">
-        <v>300</v>
-      </c>
-      <c r="C4" t="s">
-        <v>202</v>
-      </c>
-      <c r="E4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>221</v>
       </c>
       <c r="B5">
-        <v>-6</v>
+        <v>-30</v>
       </c>
       <c r="C5" t="s">
         <v>190</v>
@@ -1520,15 +1559,18 @@
         <v>196</v>
       </c>
       <c r="E5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="F5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>223</v>
       </c>
       <c r="B6">
-        <v>-15</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>190</v>
@@ -1537,32 +1579,35 @@
         <v>196</v>
       </c>
       <c r="E6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+      <c r="F6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B7">
-        <v>-4.9000000000000004</v>
+        <v>300</v>
       </c>
       <c r="C7" t="s">
-        <v>190</v>
-      </c>
-      <c r="D7" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="E7" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+      <c r="F7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B8">
-        <v>0.2</v>
+        <v>-6</v>
       </c>
       <c r="C8" t="s">
         <v>190</v>
@@ -1571,24 +1616,70 @@
         <v>196</v>
       </c>
       <c r="E8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+      <c r="F8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B9">
-        <v>0.01</v>
+        <v>-15</v>
       </c>
       <c r="C9" t="s">
         <v>190</v>
       </c>
       <c r="D9" t="s">
-        <v>88</v>
+        <v>196</v>
       </c>
       <c r="E9" t="s">
-        <v>205</v>
+        <v>198</v>
+      </c>
+      <c r="F9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="C10" t="s">
+        <v>190</v>
+      </c>
+      <c r="D10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E10" t="s">
+        <v>199</v>
+      </c>
+      <c r="F10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>195</v>
+      </c>
+      <c r="B11">
+        <v>0.2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D11" t="s">
+        <v>196</v>
+      </c>
+      <c r="E11" t="s">
+        <v>200</v>
+      </c>
+      <c r="F11" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -1684,7 +1775,7 @@
       <c r="J2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="K2" s="15" t="b">
+      <c r="K2" s="2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove accel filter in detect_kneepoint
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8EF05A-F0D2-0A41-935B-F81098573E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0784476B-D3FD-AA44-868C-3EB341312E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="800" windowWidth="34200" windowHeight="20320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="228">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -720,6 +720,9 @@
   </si>
   <si>
     <t>InputHandler</t>
+  </si>
+  <si>
+    <t>CUTOFF_FREQ</t>
   </si>
 </sst>
 </file>
@@ -1451,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1507,30 +1510,24 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F3" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>190</v>
@@ -1539,7 +1536,7 @@
         <v>88</v>
       </c>
       <c r="E4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F4" t="s">
         <v>220</v>
@@ -1547,19 +1544,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="B5">
-        <v>-30</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>190</v>
       </c>
       <c r="D5" t="s">
-        <v>196</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="F5" t="s">
         <v>220</v>
@@ -1567,10 +1564,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B6">
-        <v>29</v>
+        <v>-30</v>
       </c>
       <c r="C6" t="s">
         <v>190</v>
@@ -1579,7 +1576,7 @@
         <v>196</v>
       </c>
       <c r="E6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F6" t="s">
         <v>220</v>
@@ -1587,36 +1584,36 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
       <c r="B7">
-        <v>300</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>202</v>
+        <v>190</v>
+      </c>
+      <c r="D7" t="s">
+        <v>196</v>
       </c>
       <c r="E7" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="F7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B8">
-        <v>-6</v>
+        <v>300</v>
       </c>
       <c r="C8" t="s">
-        <v>190</v>
-      </c>
-      <c r="D8" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="E8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="F8" t="s">
         <v>225</v>
@@ -1624,10 +1621,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B9">
-        <v>-15</v>
+        <v>-6</v>
       </c>
       <c r="C9" t="s">
         <v>190</v>
@@ -1636,7 +1633,7 @@
         <v>196</v>
       </c>
       <c r="E9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F9" t="s">
         <v>225</v>
@@ -1644,10 +1641,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B10">
-        <v>-4.9000000000000004</v>
+        <v>-15</v>
       </c>
       <c r="C10" t="s">
         <v>190</v>
@@ -1656,7 +1653,7 @@
         <v>196</v>
       </c>
       <c r="E10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F10" t="s">
         <v>225</v>
@@ -1664,10 +1661,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B11">
-        <v>0.2</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="C11" t="s">
         <v>190</v>
@@ -1676,15 +1673,36 @@
         <v>196</v>
       </c>
       <c r="E11" t="s">
+        <v>199</v>
+      </c>
+      <c r="F11" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12">
+        <v>0.2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D12" t="s">
+        <v>196</v>
+      </c>
+      <c r="E12" t="s">
         <v>200</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>225</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
polish the remaining accel filter logic shift
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0784476B-D3FD-AA44-868C-3EB341312E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82BE9DA-ED89-994C-BD0F-4BFAF06AC643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="800" windowWidth="34200" windowHeight="20320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="34200" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="234">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -723,6 +723,24 @@
   </si>
   <si>
     <t>CUTOFF_FREQ</t>
+  </si>
+  <si>
+    <t>aebRequest</t>
+  </si>
+  <si>
+    <t>fcw_request</t>
+  </si>
+  <si>
+    <t>fcwRequest</t>
+  </si>
+  <si>
+    <t>aeb_request</t>
+  </si>
+  <si>
+    <t>dbs_request</t>
+  </si>
+  <si>
+    <t>dbsRequest</t>
   </si>
 </sst>
 </file>
@@ -1161,9 +1179,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1361,19 +1379,37 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
+      <c r="A18" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
+      <c r="A19" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
+      <c r="A20" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
@@ -1456,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
encode categorical MDF channels numerically with NV enums
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82BE9DA-ED89-994C-BD0F-4BFAF06AC643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894A56EE-DCDD-8A47-BC43-5342D9C68D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="800" windowWidth="34200" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="235">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -741,6 +741,9 @@
   </si>
   <si>
     <t>dbsRequest</t>
+  </si>
+  <si>
+    <t>enum</t>
   </si>
 </sst>
 </file>
@@ -1177,11 +1180,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1191,7 +1194,7 @@
     <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>47</v>
       </c>
@@ -1201,8 +1204,11 @@
       <c r="C1" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1212,8 +1218,11 @@
       <c r="C2" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1223,8 +1232,11 @@
       <c r="C3" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1234,8 +1246,11 @@
       <c r="C4" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>96</v>
       </c>
@@ -1245,8 +1260,11 @@
       <c r="C5" s="6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>96</v>
       </c>
@@ -1256,8 +1274,11 @@
       <c r="C6" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -1267,8 +1288,11 @@
       <c r="C7" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
@@ -1278,8 +1302,11 @@
       <c r="C8" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>96</v>
       </c>
@@ -1289,8 +1316,11 @@
       <c r="C9" s="6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -1300,8 +1330,11 @@
       <c r="C10" s="6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>2</v>
       </c>
@@ -1311,8 +1344,11 @@
       <c r="C11" s="6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
@@ -1322,8 +1358,11 @@
       <c r="C12" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
@@ -1333,8 +1372,11 @@
       <c r="C13" s="6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
@@ -1344,8 +1386,11 @@
       <c r="C14" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -1355,8 +1400,11 @@
       <c r="C15" s="6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>28</v>
       </c>
@@ -1366,8 +1414,11 @@
       <c r="C16" s="6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -1377,8 +1428,11 @@
       <c r="C17" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>228</v>
       </c>
@@ -1388,8 +1442,11 @@
       <c r="C18" s="9" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>228</v>
       </c>
@@ -1399,8 +1456,11 @@
       <c r="C19" s="9" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>228</v>
       </c>
@@ -1410,63 +1470,66 @@
       <c r="C20" s="9" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="8"/>
       <c r="C30" s="9"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="B31" s="8"/>
       <c r="C31" s="9"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="8"/>
       <c r="C32" s="9"/>

</xml_diff>

<commit_message>
remove prefix of kpi_ in aeb kpi calculation files
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894A56EE-DCDD-8A47-BC43-5342D9C68D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A1955A-435D-CD48-BC87-940E80EE1A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="800" windowWidth="34200" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1640" yWindow="4860" windowWidth="31420" windowHeight="14360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -644,9 +644,6 @@
     <t>Tolerance for target deceleration</t>
   </si>
   <si>
-    <t>RE-SAMPLE</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -744,6 +741,9 @@
   </si>
   <si>
     <t>enum</t>
+  </si>
+  <si>
+    <t>RESAMPLE_RATE</t>
   </si>
 </sst>
 </file>
@@ -1182,9 +1182,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1401,7 +1401,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1415,7 +1415,7 @@
         <v>66</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1429,49 +1429,49 @@
         <v>182</v>
       </c>
       <c r="D17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>230</v>
-      </c>
       <c r="D18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" t="s">
         <v>233</v>
-      </c>
-      <c r="D20" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1555,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1584,12 +1584,12 @@
         <v>185</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>234</v>
       </c>
       <c r="B2">
         <v>0.01</v>
@@ -1601,24 +1601,24 @@
         <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1635,10 +1635,10 @@
         <v>88</v>
       </c>
       <c r="E4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1655,15 +1655,15 @@
         <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B6">
         <v>-30</v>
@@ -1675,15 +1675,15 @@
         <v>196</v>
       </c>
       <c r="E6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B7">
         <v>29</v>
@@ -1695,10 +1695,10 @@
         <v>196</v>
       </c>
       <c r="E7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1709,13 +1709,13 @@
         <v>300</v>
       </c>
       <c r="C8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1735,7 +1735,7 @@
         <v>197</v>
       </c>
       <c r="F9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1755,7 +1755,7 @@
         <v>198</v>
       </c>
       <c r="F10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1775,7 +1775,7 @@
         <v>199</v>
       </c>
       <c r="F11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1795,7 +1795,7 @@
         <v>200</v>
       </c>
       <c r="F12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -1858,7 +1858,7 @@
         <v>81</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1968,7 +1968,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>178</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>179</v>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>24</v>
@@ -3043,7 +3043,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>93</v>
@@ -3055,7 +3055,7 @@
         <v>95</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
@@ -3072,7 +3072,7 @@
         <v>0.70499999999999996</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
@@ -3089,7 +3089,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
@@ -3106,7 +3106,7 @@
         <v>0.17199999999999999</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
@@ -3123,7 +3123,7 @@
         <v>0.157</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
@@ -3140,7 +3140,7 @@
         <v>0.74099999999999999</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
@@ -3157,7 +3157,7 @@
         <v>0.29399999999999998</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
@@ -3174,7 +3174,7 @@
         <v>0.76</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make kpi_table builder feature-aware
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A1955A-435D-CD48-BC87-940E80EE1A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D341E79F-9406-B440-917A-ECA6620FBA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="4860" windowWidth="31420" windowHeight="14360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1640" yWindow="4860" windowWidth="31420" windowHeight="14360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="246">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -744,6 +744,39 @@
   </si>
   <si>
     <t>RESAMPLE_RATE</t>
+  </si>
+  <si>
+    <t>FCW</t>
+  </si>
+  <si>
+    <t>req-5256401-00186197</t>
+  </si>
+  <si>
+    <t>brakeJerkDur</t>
+  </si>
+  <si>
+    <t>duration of haptic warning</t>
+  </si>
+  <si>
+    <t>peakJerk</t>
+  </si>
+  <si>
+    <t>peakDecel</t>
+  </si>
+  <si>
+    <t>req-5256401-00193880</t>
+  </si>
+  <si>
+    <t>req-5256401-00202186</t>
+  </si>
+  <si>
+    <t>m/s³</t>
+  </si>
+  <si>
+    <t>max jerk during brake jerk event</t>
+  </si>
+  <si>
+    <t>max deceleration during brake jerk event</t>
   </si>
 </sst>
 </file>
@@ -1555,7 +1588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -2321,11 +2354,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE39B99-0AFB-8547-83BF-D855CC6E3BB3}">
-  <dimension ref="B1:G35"/>
+  <dimension ref="B1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2960,6 +2993,66 @@
       <c r="F35" s="12"/>
       <c r="G35" s="12" t="s">
         <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F36" t="s">
+        <v>236</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B37" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="F37" t="s">
+        <v>241</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B38" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F38" t="s">
+        <v>242</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify kpi_table builder to always include Common KPIs automatically
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D341E79F-9406-B440-917A-ECA6620FBA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E859015-2089-6645-A604-06F10A8C30D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="4860" windowWidth="31420" windowHeight="14360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="700" windowWidth="34140" windowHeight="20420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="250">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -777,6 +777,18 @@
   </si>
   <si>
     <t>max deceleration during brake jerk event</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>name of the mdf chunk</t>
   </si>
 </sst>
 </file>
@@ -869,7 +881,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -899,6 +911,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1843,7 +1856,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2354,17 +2367,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE39B99-0AFB-8547-83BF-D855CC6E3BB3}">
-  <dimension ref="B1:G38"/>
+  <dimension ref="B1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J39" sqref="J39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
@@ -2392,58 +2405,56 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
-        <v>130</v>
+        <v>246</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>108</v>
+        <v>247</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>88</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12" t="s">
-        <v>133</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
-        <v>130</v>
+        <v>246</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
-        <v>130</v>
+        <v>246</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>173</v>
+        <v>29</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
@@ -2451,7 +2462,7 @@
         <v>130</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>109</v>
@@ -2461,7 +2472,7 @@
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
@@ -2469,7 +2480,7 @@
         <v>130</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>109</v>
@@ -2479,7 +2490,7 @@
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
@@ -2487,7 +2498,7 @@
         <v>130</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>109</v>
@@ -2497,7 +2508,7 @@
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
@@ -2505,7 +2516,7 @@
         <v>130</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>30</v>
+        <v>176</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>109</v>
@@ -2515,7 +2526,7 @@
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
@@ -2523,15 +2534,17 @@
         <v>130</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" s="12"/>
+        <v>109</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>88</v>
+      </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
@@ -2539,7 +2552,7 @@
         <v>130</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>112</v>
+        <v>36</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>111</v>
@@ -2547,7 +2560,7 @@
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
@@ -2555,7 +2568,7 @@
         <v>130</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>111</v>
@@ -2563,7 +2576,7 @@
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
@@ -2571,17 +2584,15 @@
         <v>130</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>88</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
@@ -2589,7 +2600,7 @@
         <v>130</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>109</v>
@@ -2599,7 +2610,7 @@
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
@@ -2607,17 +2618,17 @@
         <v>130</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>177</v>
+        <v>115</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
@@ -2625,15 +2636,17 @@
         <v>130</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>117</v>
+        <v>177</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" s="12"/>
+        <v>109</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>116</v>
+      </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
@@ -2641,17 +2654,15 @@
         <v>130</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>178</v>
+        <v>117</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>116</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
@@ -2659,7 +2670,7 @@
         <v>130</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>109</v>
@@ -2669,7 +2680,7 @@
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
@@ -2677,7 +2688,7 @@
         <v>130</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>118</v>
+        <v>179</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>109</v>
@@ -2685,11 +2696,9 @@
       <c r="E18" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="12" t="s">
-        <v>172</v>
-      </c>
+      <c r="F18" s="12"/>
       <c r="G18" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
@@ -2697,15 +2706,19 @@
         <v>130</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>180</v>
+        <v>118</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+        <v>109</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>172</v>
+      </c>
       <c r="G19" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
@@ -2713,17 +2726,15 @@
         <v>130</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>31</v>
+        <v>180</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>119</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
@@ -2731,7 +2742,7 @@
         <v>130</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>120</v>
+        <v>31</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>109</v>
@@ -2739,11 +2750,9 @@
       <c r="E21" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="F21" s="12" t="s">
-        <v>170</v>
-      </c>
+      <c r="F21" s="12"/>
       <c r="G21" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
@@ -2751,15 +2760,19 @@
         <v>130</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+        <v>109</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>170</v>
+      </c>
       <c r="G22" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
@@ -2767,17 +2780,15 @@
         <v>130</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>122</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
@@ -2785,7 +2796,7 @@
         <v>130</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>123</v>
+        <v>32</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>109</v>
@@ -2793,11 +2804,9 @@
       <c r="E24" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="F24" s="12" t="s">
-        <v>171</v>
-      </c>
+      <c r="F24" s="12"/>
       <c r="G24" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
@@ -2805,15 +2814,19 @@
         <v>130</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+        <v>109</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>171</v>
+      </c>
       <c r="G25" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
@@ -2821,17 +2834,15 @@
         <v>130</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>157</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
@@ -2839,7 +2850,7 @@
         <v>130</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>125</v>
+        <v>34</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>109</v>
@@ -2847,11 +2858,9 @@
       <c r="E27" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="F27" s="12" t="s">
-        <v>169</v>
-      </c>
+      <c r="F27" s="12"/>
       <c r="G27" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
@@ -2859,15 +2868,19 @@
         <v>130</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+        <v>109</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>169</v>
+      </c>
       <c r="G28" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
@@ -2875,16 +2888,15 @@
         <v>130</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>122</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
       <c r="G29" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
@@ -2892,7 +2904,7 @@
         <v>130</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>127</v>
+        <v>33</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>109</v>
@@ -2900,11 +2912,8 @@
       <c r="E30" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="F30" s="12" t="s">
-        <v>168</v>
-      </c>
       <c r="G30" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
@@ -2912,15 +2921,19 @@
         <v>130</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
+        <v>109</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>168</v>
+      </c>
       <c r="G31" s="12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
@@ -2928,17 +2941,15 @@
         <v>130</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>129</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
@@ -2946,7 +2957,7 @@
         <v>130</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>109</v>
@@ -2956,7 +2967,7 @@
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
@@ -2964,7 +2975,7 @@
         <v>130</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>109</v>
@@ -2974,7 +2985,7 @@
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
@@ -2982,7 +2993,7 @@
         <v>130</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>109</v>
@@ -2992,27 +3003,25 @@
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" s="12" t="s">
-        <v>235</v>
+        <v>130</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>237</v>
+        <v>79</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F36" t="s">
-        <v>236</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="F36" s="12"/>
       <c r="G36" s="12" t="s">
-        <v>238</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
@@ -3020,19 +3029,19 @@
         <v>235</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>243</v>
+        <v>88</v>
       </c>
       <c r="F37" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
@@ -3040,18 +3049,38 @@
         <v>235</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E38" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="F38" t="s">
+        <v>241</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B39" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>242</v>
       </c>
-      <c r="G38" s="12" t="s">
+      <c r="G39" s="12" t="s">
         <v>245</v>
       </c>
     </row>

</xml_diff>

<commit_message>
make event_detector,kpi_extractor,visualizer and visualizer feature specific
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E859015-2089-6645-A604-06F10A8C30D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7A0D86-D503-144D-9ECE-39A090CF03EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="700" windowWidth="34140" windowHeight="20420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="700" windowWidth="34140" windowHeight="20420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="255">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -713,9 +713,6 @@
     <t># threshold for positive change (event end)</t>
   </si>
   <si>
-    <t>KpiExtractor</t>
-  </si>
-  <si>
     <t>InputHandler</t>
   </si>
   <si>
@@ -789,6 +786,24 @@
   </si>
   <si>
     <t>name of the mdf chunk</t>
+  </si>
+  <si>
+    <t>AebKpiExtractor</t>
+  </si>
+  <si>
+    <t>FcwKpiExtractor</t>
+  </si>
+  <si>
+    <t>WINDOW_S</t>
+  </si>
+  <si>
+    <t>JERK_THD</t>
+  </si>
+  <si>
+    <t>Duration after FCW=3 rising edge to search (default 1 s).</t>
+  </si>
+  <si>
+    <t>Fixed jerk threshold. If None, uses adaptive MAD-based threshold.</t>
   </si>
 </sst>
 </file>
@@ -1447,7 +1462,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1461,7 +1476,7 @@
         <v>66</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1475,49 +1490,49 @@
         <v>182</v>
       </c>
       <c r="D17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>229</v>
-      </c>
       <c r="D18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" t="s">
         <v>232</v>
-      </c>
-      <c r="D20" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1599,17 +1614,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="4" width="8.83203125" customWidth="1"/>
-    <col min="5" max="5" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.5" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1635,7 +1650,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B2">
         <v>0.01</v>
@@ -1650,12 +1665,12 @@
         <v>204</v>
       </c>
       <c r="F2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -1664,7 +1679,7 @@
         <v>201</v>
       </c>
       <c r="F3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1761,7 +1776,7 @@
         <v>217</v>
       </c>
       <c r="F8" t="s">
-        <v>224</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1781,7 +1796,7 @@
         <v>197</v>
       </c>
       <c r="F9" t="s">
-        <v>224</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1801,7 +1816,7 @@
         <v>198</v>
       </c>
       <c r="F10" t="s">
-        <v>224</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1821,7 +1836,7 @@
         <v>199</v>
       </c>
       <c r="F11" t="s">
-        <v>224</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1841,7 +1856,44 @@
         <v>200</v>
       </c>
       <c r="F12" t="s">
-        <v>224</v>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>251</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>190</v>
+      </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" t="s">
+        <v>253</v>
+      </c>
+      <c r="F13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>252</v>
+      </c>
+      <c r="C14" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" t="s">
+        <v>242</v>
+      </c>
+      <c r="E14" t="s">
+        <v>254</v>
+      </c>
+      <c r="F14" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2369,7 +2421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE39B99-0AFB-8547-83BF-D855CC6E3BB3}">
   <dimension ref="B1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
@@ -2407,23 +2459,23 @@
     </row>
     <row r="2" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>247</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>248</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>108</v>
@@ -2441,7 +2493,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>29</v>
@@ -3026,10 +3078,10 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>109</v>
@@ -3038,38 +3090,38 @@
         <v>88</v>
       </c>
       <c r="F37" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E38" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="F38" t="s">
+        <v>240</v>
+      </c>
+      <c r="G38" s="12" t="s">
         <v>243</v>
-      </c>
-      <c r="F38" t="s">
-        <v>241</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>109</v>
@@ -3078,10 +3130,10 @@
         <v>157</v>
       </c>
       <c r="F39" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename event_detector to event_segmenter and move event-detection logic to a standalone reusable function.
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17EA6DE-05F3-9A47-9FB8-2319331D6F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2908D872-4A00-7D44-8474-2EEB5113AA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="700" windowWidth="34140" windowHeight="20420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="700" windowWidth="34140" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="259">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -692,9 +692,6 @@
     <t>Class</t>
   </si>
   <si>
-    <t>EventDetector</t>
-  </si>
-  <si>
     <t>START_DECEL_DELTA</t>
   </si>
   <si>
@@ -749,12 +746,6 @@
     <t>duration of haptic warning</t>
   </si>
   <si>
-    <t>peakJerk</t>
-  </si>
-  <si>
-    <t>peakDecel</t>
-  </si>
-  <si>
     <t>req-5256401-00193880</t>
   </si>
   <si>
@@ -804,6 +795,27 @@
   </si>
   <si>
     <t>POST_TIME_FCW</t>
+  </si>
+  <si>
+    <t>FcwEventDetector</t>
+  </si>
+  <si>
+    <t>AebEventDetector</t>
+  </si>
+  <si>
+    <t>brakeJerkStart</t>
+  </si>
+  <si>
+    <t>brakeJerkEnd</t>
+  </si>
+  <si>
+    <t>brakeJerkThd</t>
+  </si>
+  <si>
+    <t>brakeJerkMax</t>
+  </si>
+  <si>
+    <t>brakeAccelMax</t>
   </si>
 </sst>
 </file>
@@ -896,7 +908,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -926,7 +938,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1243,7 +1254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -1462,7 +1473,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1476,7 +1487,7 @@
         <v>66</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1490,49 +1501,49 @@
         <v>182</v>
       </c>
       <c r="D17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>226</v>
-      </c>
       <c r="D18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" t="s">
         <v>229</v>
-      </c>
-      <c r="D20" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1616,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1625,7 +1636,7 @@
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="4" width="8.83203125" customWidth="1"/>
     <col min="5" max="5" width="66.5" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -1650,7 +1661,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B2">
         <v>0.01</v>
@@ -1665,12 +1676,12 @@
         <v>202</v>
       </c>
       <c r="F2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -1679,12 +1690,12 @@
         <v>199</v>
       </c>
       <c r="F3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B4">
         <v>-30</v>
@@ -1696,15 +1707,15 @@
         <v>194</v>
       </c>
       <c r="E4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F4" t="s">
-        <v>217</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B5">
         <v>29</v>
@@ -1716,10 +1727,10 @@
         <v>194</v>
       </c>
       <c r="E5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F5" t="s">
-        <v>217</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1736,7 +1747,7 @@
         <v>215</v>
       </c>
       <c r="F6" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1756,7 +1767,7 @@
         <v>195</v>
       </c>
       <c r="F7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1776,7 +1787,7 @@
         <v>196</v>
       </c>
       <c r="F8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1796,7 +1807,7 @@
         <v>197</v>
       </c>
       <c r="F9" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1816,12 +1827,12 @@
         <v>198</v>
       </c>
       <c r="F10" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -1836,12 +1847,12 @@
         <v>200</v>
       </c>
       <c r="F11" t="s">
-        <v>217</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -1856,12 +1867,12 @@
         <v>201</v>
       </c>
       <c r="F12" t="s">
-        <v>217</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1873,27 +1884,27 @@
         <v>88</v>
       </c>
       <c r="E13" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F13" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C14" t="s">
         <v>188</v>
       </c>
       <c r="D14" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E14" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -2419,11 +2430,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE39B99-0AFB-8547-83BF-D855CC6E3BB3}">
-  <dimension ref="B1:G39"/>
+  <dimension ref="B1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2457,25 +2468,25 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>108</v>
@@ -2493,7 +2504,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>29</v>
@@ -3078,10 +3089,10 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>109</v>
@@ -3090,50 +3101,95 @@
         <v>88</v>
       </c>
       <c r="F37" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="F38" t="s">
-        <v>238</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>241</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="G38" s="12"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G39" s="12"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B40" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B41" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="F41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B42" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F42" t="s">
+        <v>236</v>
+      </c>
+      <c r="G42" s="12" t="s">
         <v>239</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3206,7 +3262,7 @@
   <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
brake jerk related kpis extracted
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2908D872-4A00-7D44-8474-2EEB5113AA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A69C13-59E1-5E43-92F7-D6035DC620F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="700" windowWidth="34140" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="700" windowWidth="34140" windowHeight="20420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="263">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -623,9 +623,6 @@
     <t>TGT_TOL</t>
   </si>
   <si>
-    <t>m/s2</t>
-  </si>
-  <si>
     <t>Target deceleration for PB in m/s²</t>
   </si>
   <si>
@@ -782,15 +779,9 @@
     <t>WINDOW_S</t>
   </si>
   <si>
-    <t>JERK_THD</t>
-  </si>
-  <si>
     <t>Duration after FCW=3 rising edge to search (default 1 s).</t>
   </si>
   <si>
-    <t>Fixed jerk threshold. If None, uses adaptive MAD-based threshold.</t>
-  </si>
-  <si>
     <t>PRE_TIME_FCW</t>
   </si>
   <si>
@@ -809,13 +800,34 @@
     <t>brakeJerkEnd</t>
   </si>
   <si>
-    <t>brakeJerkThd</t>
-  </si>
-  <si>
     <t>brakeJerkMax</t>
   </si>
   <si>
-    <t>brakeAccelMax</t>
+    <t>brakeAccelMin</t>
+  </si>
+  <si>
+    <t>JERK_NEG_THD</t>
+  </si>
+  <si>
+    <t>JERK_POS_THD</t>
+  </si>
+  <si>
+    <t>Negative jerk threshold</t>
+  </si>
+  <si>
+    <t>Positive jerk threshold</t>
+  </si>
+  <si>
+    <t>BRAKEJERK_MIN_SPEED</t>
+  </si>
+  <si>
+    <t>BRAKEJERK_MAX_SPEED</t>
+  </si>
+  <si>
+    <t>minimum speed threshold for brake jerk warning</t>
+  </si>
+  <si>
+    <t>maximum speed threshold for brake jerk warning</t>
   </si>
 </sst>
 </file>
@@ -1254,7 +1266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -1473,7 +1485,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1487,7 +1499,7 @@
         <v>66</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1501,49 +1513,49 @@
         <v>182</v>
       </c>
       <c r="D17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>225</v>
-      </c>
       <c r="D18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" t="s">
         <v>228</v>
-      </c>
-      <c r="D20" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1625,15 +1637,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="4" width="8.83203125" customWidth="1"/>
     <col min="5" max="5" width="66.5" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
@@ -1656,12 +1668,12 @@
         <v>185</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B2">
         <v>0.01</v>
@@ -1673,29 +1685,29 @@
         <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B4">
         <v>-30</v>
@@ -1704,18 +1716,18 @@
         <v>188</v>
       </c>
       <c r="D4" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="E4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B5">
         <v>29</v>
@@ -1724,13 +1736,13 @@
         <v>188</v>
       </c>
       <c r="D5" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="E5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1741,13 +1753,13 @@
         <v>300</v>
       </c>
       <c r="C6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1761,13 +1773,13 @@
         <v>188</v>
       </c>
       <c r="D7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" t="s">
         <v>194</v>
       </c>
-      <c r="E7" t="s">
-        <v>195</v>
-      </c>
       <c r="F7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1781,13 +1793,13 @@
         <v>188</v>
       </c>
       <c r="D8" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="E8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1801,13 +1813,13 @@
         <v>188</v>
       </c>
       <c r="D9" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="E9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1821,18 +1833,18 @@
         <v>188</v>
       </c>
       <c r="D10" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="E10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -1844,15 +1856,15 @@
         <v>88</v>
       </c>
       <c r="E11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F11" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -1864,15 +1876,15 @@
         <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1884,27 +1896,90 @@
         <v>88</v>
       </c>
       <c r="E13" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>247</v>
+        <v>255</v>
+      </c>
+      <c r="B14">
+        <v>-20</v>
       </c>
       <c r="C14" t="s">
         <v>188</v>
       </c>
       <c r="D14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E14" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="F14" t="s">
-        <v>245</v>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D15" t="s">
+        <v>236</v>
+      </c>
+      <c r="E15" t="s">
+        <v>258</v>
+      </c>
+      <c r="F15" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>259</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>188</v>
+      </c>
+      <c r="D16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" t="s">
+        <v>261</v>
+      </c>
+      <c r="F16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>260</v>
+      </c>
+      <c r="B17">
+        <v>130</v>
+      </c>
+      <c r="C17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" t="s">
+        <v>262</v>
+      </c>
+      <c r="F17" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -1967,7 +2042,7 @@
         <v>81</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -2077,7 +2152,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>178</v>
@@ -2112,7 +2187,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>179</v>
@@ -2131,7 +2206,7 @@
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>24</v>
@@ -2430,11 +2505,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE39B99-0AFB-8547-83BF-D855CC6E3BB3}">
-  <dimension ref="B1:G42"/>
+  <dimension ref="B1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F46" sqref="F46"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2470,23 +2545,23 @@
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>241</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>242</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>108</v>
@@ -2504,7 +2579,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>29</v>
@@ -3089,10 +3164,10 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>109</v>
@@ -3101,18 +3176,18 @@
         <v>88</v>
       </c>
       <c r="F37" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>109</v>
@@ -3124,10 +3199,10 @@
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>109</v>
@@ -3139,57 +3214,42 @@
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="G40" s="12"/>
+        <v>236</v>
+      </c>
+      <c r="F40" t="s">
+        <v>234</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>237</v>
+        <v>157</v>
       </c>
       <c r="F41" t="s">
         <v>235</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B42" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="F42" t="s">
-        <v>236</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -3273,7 +3333,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>93</v>
@@ -3285,7 +3345,7 @@
         <v>95</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
@@ -3302,7 +3362,7 @@
         <v>0.70499999999999996</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
@@ -3319,7 +3379,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
@@ -3336,7 +3396,7 @@
         <v>0.17199999999999999</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
@@ -3353,7 +3413,7 @@
         <v>0.157</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
@@ -3370,7 +3430,7 @@
         <v>0.74099999999999999</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
@@ -3387,7 +3447,7 @@
         <v>0.29399999999999998</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
@@ -3404,7 +3464,7 @@
         <v>0.76</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
load aeb relevant params from class and config
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A69C13-59E1-5E43-92F7-D6035DC620F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8A8C8A-6506-2241-88C0-15F677EB740E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="700" windowWidth="34140" windowHeight="20420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38160" yWindow="6440" windowWidth="38400" windowHeight="20980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="267">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -782,15 +782,6 @@
     <t>Duration after FCW=3 rising edge to search (default 1 s).</t>
   </si>
   <si>
-    <t>PRE_TIME_FCW</t>
-  </si>
-  <si>
-    <t>POST_TIME_FCW</t>
-  </si>
-  <si>
-    <t>FcwEventDetector</t>
-  </si>
-  <si>
     <t>AebEventDetector</t>
   </si>
   <si>
@@ -828,6 +819,27 @@
   </si>
   <si>
     <t>maximum speed threshold for brake jerk warning</t>
+  </si>
+  <si>
+    <t>PRE_TIME_DEFAULT</t>
+  </si>
+  <si>
+    <t>POST_TIME_DEFAULT</t>
+  </si>
+  <si>
+    <t>default time before event (duration)</t>
+  </si>
+  <si>
+    <t>default time after event (duration)</t>
+  </si>
+  <si>
+    <t>BaseEventSegmenter</t>
+  </si>
+  <si>
+    <t>PRE_TIME_AEB</t>
+  </si>
+  <si>
+    <t>POST_TIME_AEB</t>
   </si>
 </sst>
 </file>
@@ -1637,10 +1649,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1707,67 +1719,70 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>265</v>
       </c>
       <c r="B4">
-        <v>-30</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>188</v>
       </c>
       <c r="D4" t="s">
-        <v>157</v>
+        <v>88</v>
       </c>
       <c r="E4" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="F4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>218</v>
+        <v>266</v>
       </c>
       <c r="B5">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>188</v>
       </c>
       <c r="D5" t="s">
-        <v>157</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="F5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="B6">
-        <v>300</v>
+        <v>-30</v>
       </c>
       <c r="C6" t="s">
-        <v>198</v>
+        <v>188</v>
+      </c>
+      <c r="D6" t="s">
+        <v>157</v>
       </c>
       <c r="E6" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F6" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>218</v>
       </c>
       <c r="B7">
-        <v>-6</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>188</v>
@@ -1776,27 +1791,24 @@
         <v>157</v>
       </c>
       <c r="E7" t="s">
-        <v>194</v>
+        <v>219</v>
       </c>
       <c r="F7" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B8">
-        <v>-15</v>
+        <v>300</v>
       </c>
       <c r="C8" t="s">
-        <v>188</v>
-      </c>
-      <c r="D8" t="s">
-        <v>157</v>
+        <v>198</v>
       </c>
       <c r="E8" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="F8" t="s">
         <v>243</v>
@@ -1804,10 +1816,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B9">
-        <v>-4.9000000000000004</v>
+        <v>-6</v>
       </c>
       <c r="C9" t="s">
         <v>188</v>
@@ -1816,7 +1828,7 @@
         <v>157</v>
       </c>
       <c r="E9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F9" t="s">
         <v>243</v>
@@ -1824,10 +1836,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B10">
-        <v>0.2</v>
+        <v>-15</v>
       </c>
       <c r="C10" t="s">
         <v>188</v>
@@ -1836,7 +1848,7 @@
         <v>157</v>
       </c>
       <c r="E10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F10" t="s">
         <v>243</v>
@@ -1844,42 +1856,42 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>192</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="C11" t="s">
         <v>188</v>
       </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
       <c r="E11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F11" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>248</v>
+        <v>193</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>0.2</v>
       </c>
       <c r="C12" t="s">
         <v>188</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
       <c r="E12" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F12" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1904,7 +1916,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B14">
         <v>-20</v>
@@ -1916,7 +1928,7 @@
         <v>236</v>
       </c>
       <c r="E14" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F14" t="s">
         <v>244</v>
@@ -1924,7 +1936,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B15">
         <v>20</v>
@@ -1936,7 +1948,7 @@
         <v>236</v>
       </c>
       <c r="E15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F15" t="s">
         <v>244</v>
@@ -1944,7 +1956,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B16">
         <v>30</v>
@@ -1956,7 +1968,7 @@
         <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F16" t="s">
         <v>244</v>
@@ -1964,7 +1976,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -1976,10 +1988,50 @@
         <v>110</v>
       </c>
       <c r="E17" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F17" t="s">
         <v>244</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>260</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>188</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" t="s">
+        <v>262</v>
+      </c>
+      <c r="F18" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>188</v>
+      </c>
+      <c r="D19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F19" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -3187,7 +3239,7 @@
         <v>230</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>109</v>
@@ -3202,7 +3254,7 @@
         <v>230</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>109</v>
@@ -3217,7 +3269,7 @@
         <v>230</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>109</v>
@@ -3237,7 +3289,7 @@
         <v>230</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
fix pre and post time loading for FcwEventSegmenter
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8A8C8A-6506-2241-88C0-15F677EB740E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3813EE-4C91-BE46-A992-AFC355091CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38160" yWindow="6440" windowWidth="38400" windowHeight="20980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="270">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -780,6 +780,15 @@
   </si>
   <si>
     <t>Duration after FCW=3 rising edge to search (default 1 s).</t>
+  </si>
+  <si>
+    <t>PRE_TIME_FCW</t>
+  </si>
+  <si>
+    <t>POST_TIME_FCW</t>
+  </si>
+  <si>
+    <t>FcwEventDetector</t>
   </si>
   <si>
     <t>AebEventDetector</t>
@@ -1649,10 +1658,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1719,7 +1728,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -1734,12 +1743,12 @@
         <v>199</v>
       </c>
       <c r="F4" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1754,7 +1763,7 @@
         <v>200</v>
       </c>
       <c r="F5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1774,7 +1783,7 @@
         <v>217</v>
       </c>
       <c r="F6" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1794,7 +1803,7 @@
         <v>219</v>
       </c>
       <c r="F7" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1896,10 +1905,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
         <v>188</v>
@@ -1908,47 +1917,47 @@
         <v>88</v>
       </c>
       <c r="E13" t="s">
-        <v>246</v>
+        <v>199</v>
       </c>
       <c r="F13" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B14">
-        <v>-20</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
         <v>188</v>
       </c>
       <c r="D14" t="s">
-        <v>236</v>
+        <v>88</v>
       </c>
       <c r="E14" t="s">
-        <v>254</v>
+        <v>200</v>
       </c>
       <c r="F14" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B15">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
         <v>188</v>
       </c>
       <c r="D15" t="s">
-        <v>236</v>
+        <v>88</v>
       </c>
       <c r="E15" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="F15" t="s">
         <v>244</v>
@@ -1956,19 +1965,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B16">
-        <v>30</v>
+        <v>-20</v>
       </c>
       <c r="C16" t="s">
         <v>188</v>
       </c>
       <c r="D16" t="s">
-        <v>110</v>
+        <v>236</v>
       </c>
       <c r="E16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F16" t="s">
         <v>244</v>
@@ -1976,19 +1985,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B17">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>188</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>236</v>
       </c>
       <c r="E17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F17" t="s">
         <v>244</v>
@@ -1996,42 +2005,82 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>188</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="E18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F18" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>130</v>
       </c>
       <c r="C19" t="s">
         <v>188</v>
       </c>
       <c r="D19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" t="s">
+        <v>262</v>
+      </c>
+      <c r="F19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>263</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>188</v>
+      </c>
+      <c r="D20" t="s">
         <v>88</v>
       </c>
-      <c r="E19" t="s">
-        <v>263</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E20" t="s">
+        <v>265</v>
+      </c>
+      <c r="F20" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>264</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" t="s">
+        <v>266</v>
+      </c>
+      <c r="F21" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -3239,7 +3288,7 @@
         <v>230</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>109</v>
@@ -3254,7 +3303,7 @@
         <v>230</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>109</v>
@@ -3269,7 +3318,7 @@
         <v>230</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>109</v>
@@ -3289,7 +3338,7 @@
         <v>230</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
refactored AebKpiExtractor and FcwKpiExtractor
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3813EE-4C91-BE46-A992-AFC355091CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48CA419-50B8-6B4F-9BA2-D6E8495E3308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38160" yWindow="6440" windowWidth="38400" windowHeight="20980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38240" yWindow="4860" windowWidth="34200" windowHeight="20480" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -1660,8 +1660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1669,7 +1669,7 @@
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="4" width="8.83203125" customWidth="1"/>
     <col min="5" max="5" width="66.5" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -2608,9 +2608,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE39B99-0AFB-8547-83BF-D855CC6E3BB3}">
   <dimension ref="B1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fcw warning ttc metric added
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DD2592-DC30-2048-A270-5802ED4E6FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DA3242-C6EF-7543-81E2-01FFBE768554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="20400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="291">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -227,9 +227,6 @@
     <t>aeb_state_info/time_to_collision</t>
   </si>
   <si>
-    <t>ttc</t>
-  </si>
-  <si>
     <t>aeb_state_info/aeb_full_state_info/state</t>
   </si>
   <si>
@@ -873,6 +870,53 @@
   </si>
   <si>
     <t>Min Brake Acceleration</t>
+  </si>
+  <si>
+    <t>DIStatus</t>
+  </si>
+  <si>
+    <t>active_safety_status/settings/FCW/configuration_level</t>
+  </si>
+  <si>
+    <t>fcwSensitivity</t>
+  </si>
+  <si>
+    <t>aebTTC</t>
+  </si>
+  <si>
+    <t>fcwTTC</t>
+  </si>
+  <si>
+    <t>fcw_state_info/time_to_collision</t>
+  </si>
+  <si>
+    <t>req-5256401-00186185
+req-5256401-00186186
+req-5256401-00186188
+req-5256401-00186191
+req-5256401-00186192
+req-5256401-00186193</t>
+  </si>
+  <si>
+    <t>warning activation timing</t>
+  </si>
+  <si>
+    <t>FCW Warning Activation Timing</t>
+  </si>
+  <si>
+    <t>Warning Activation Timing</t>
+  </si>
+  <si>
+    <t>fcwWarningTTC</t>
+  </si>
+  <si>
+    <t>Warning TTC(s)</t>
+  </si>
+  <si>
+    <t>fcwSensitivityLvl</t>
+  </si>
+  <si>
+    <t>0: Early / 1: Normal</t>
   </si>
 </sst>
 </file>
@@ -938,7 +982,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -961,11 +1005,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -987,7 +1042,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -995,8 +1049,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1315,7 +1385,7 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1336,7 +1406,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1344,13 +1414,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>48</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1364,7 +1434,7 @@
         <v>49</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1378,12 +1448,12 @@
         <v>50</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>51</v>
@@ -1392,12 +1462,12 @@
         <v>52</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>5</v>
@@ -1406,7 +1476,7 @@
         <v>53</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1420,7 +1490,7 @@
         <v>54</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1434,12 +1504,12 @@
         <v>55</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>9</v>
@@ -1448,7 +1518,7 @@
         <v>56</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1462,7 +1532,7 @@
         <v>57</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1476,7 +1546,7 @@
         <v>58</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1490,7 +1560,7 @@
         <v>35</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1504,7 +1574,7 @@
         <v>60</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1515,10 +1585,10 @@
         <v>61</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>62</v>
+        <v>280</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1526,13 +1596,13 @@
         <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1540,80 +1610,98 @@
         <v>28</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="D16" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B17" t="s">
+        <v>180</v>
+      </c>
+      <c r="C17" t="s">
         <v>181</v>
       </c>
-      <c r="C17" t="s">
-        <v>182</v>
-      </c>
       <c r="D17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>224</v>
-      </c>
       <c r="D18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" t="s">
         <v>227</v>
       </c>
-      <c r="D20" t="s">
-        <v>228</v>
-      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
+      <c r="A21" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="D21" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
+      <c r="A22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="D22" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
@@ -1700,413 +1788,413 @@
   <sheetData>
     <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>185</v>
-      </c>
       <c r="F1" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B2">
         <v>0.01</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B4">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B6">
         <v>-30</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B7">
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B8">
         <v>300</v>
       </c>
       <c r="C8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B9">
         <v>-6</v>
       </c>
       <c r="C9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B10">
         <v>-15</v>
       </c>
       <c r="C10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B11">
         <v>-4.9000000000000004</v>
       </c>
       <c r="C11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B12">
         <v>0.2</v>
       </c>
       <c r="C12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B13">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B16">
         <v>-20</v>
       </c>
       <c r="C16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B17">
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B18">
         <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B19">
         <v>130</v>
       </c>
       <c r="C19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F19" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B20">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s">
+        <v>265</v>
+      </c>
+      <c r="F21" t="s">
         <v>266</v>
-      </c>
-      <c r="F21" t="s">
-        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -2118,10 +2206,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24310F59-1486-4F41-B3B7-AB25CE8F592D}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2139,10 +2227,10 @@
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>10</v>
@@ -2157,7 +2245,7 @@
         <v>13</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>14</v>
@@ -2169,15 +2257,15 @@
         <v>23</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>37</v>
@@ -2192,7 +2280,7 @@
         <v>85</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>16</v>
@@ -2215,13 +2303,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>175</v>
+        <v>100</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>174</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -2230,7 +2318,7 @@
         <v>0.5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" s="2" t="b">
         <v>1</v>
@@ -2253,10 +2341,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>30</v>
@@ -2268,7 +2356,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>36</v>
@@ -2291,13 +2379,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -2306,7 +2394,7 @@
         <v>100</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G5" s="2" t="b">
         <v>1</v>
@@ -2329,13 +2417,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>179</v>
+        <v>201</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>178</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -2344,14 +2432,14 @@
         <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="12" t="s">
-        <v>213</v>
+      <c r="I6" s="11" t="s">
+        <v>212</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>24</v>
@@ -2365,7 +2453,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>41</v>
@@ -2380,7 +2468,7 @@
         <v>300</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G7" s="2" t="b">
         <v>1</v>
@@ -2403,7 +2491,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>42</v>
@@ -2418,7 +2506,7 @@
         <v>600</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G8" s="2" t="b">
         <v>1</v>
@@ -2441,10 +2529,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>33</v>
@@ -2456,7 +2544,7 @@
         <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G9" s="2" t="b">
         <v>1</v>
@@ -2479,10 +2567,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>34</v>
@@ -2494,7 +2582,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G10" s="2" t="b">
         <v>1</v>
@@ -2517,13 +2605,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -2532,7 +2620,7 @@
         <v>80</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G11" s="2" t="b">
         <v>1</v>
@@ -2541,7 +2629,7 @@
         <v>17</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>24</v>
@@ -2555,13 +2643,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
@@ -2570,7 +2658,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G12" s="2" t="b">
         <v>1</v>
@@ -2579,7 +2667,7 @@
         <v>17</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>24</v>
@@ -2593,13 +2681,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="3">
         <v>0</v>
@@ -2608,7 +2696,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G13" s="2" t="b">
         <v>1</v>
@@ -2617,7 +2705,7 @@
         <v>17</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>24</v>
@@ -2631,13 +2719,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -2646,7 +2734,7 @@
         <v>5</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G14" s="2" t="b">
         <v>1</v>
@@ -2655,7 +2743,7 @@
         <v>17</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>24</v>
@@ -2669,13 +2757,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D15" s="16">
         <v>0</v>
@@ -2684,7 +2772,7 @@
         <v>0.5</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G15" s="15" t="b">
         <v>1</v>
@@ -2693,7 +2781,7 @@
         <v>17</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J15" s="15" t="s">
         <v>24</v>
@@ -2707,13 +2795,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D16" s="16">
         <v>0</v>
@@ -2722,7 +2810,7 @@
         <v>80</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G16" s="15" t="b">
         <v>1</v>
@@ -2731,7 +2819,7 @@
         <v>17</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J16" s="15" t="s">
         <v>24</v>
@@ -2745,13 +2833,13 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D17" s="16">
         <v>-6</v>
@@ -2760,7 +2848,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G17" s="15" t="b">
         <v>1</v>
@@ -2769,7 +2857,7 @@
         <v>17</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J17" s="15" t="s">
         <v>24</v>
@@ -2780,6 +2868,47 @@
       <c r="L17" s="15" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="D18" s="16">
+        <v>0</v>
+      </c>
+      <c r="E18" s="16">
+        <v>4</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="G18" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2788,751 +2917,787 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE39B99-0AFB-8547-83BF-D855CC6E3BB3}">
-  <dimension ref="B1:G41"/>
+  <dimension ref="B1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="45.1640625" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="17" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="20" customWidth="1"/>
+    <col min="7" max="7" width="45.1640625" style="20" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="C3" s="12" t="s">
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E4" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E4" s="12" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="12" t="s">
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="12" t="s">
+      <c r="D15" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12" t="s">
+      <c r="F15" s="19"/>
+      <c r="G15" s="19" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="12" t="s">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C16" s="12" t="s">
+      <c r="D17" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C18" s="12" t="s">
+      <c r="D19" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C19" s="12" t="s">
+      <c r="D20" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12" t="s">
+      <c r="F21" s="19"/>
+      <c r="G21" s="19" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E21" s="12" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12" t="s">
+      <c r="D22" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="G22" s="19" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C22" s="12" t="s">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="F22" s="12" t="s">
+      <c r="D23" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="G22" s="12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C23" s="12" t="s">
+      <c r="G25" s="19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12" t="s">
+      <c r="G30" s="19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B37" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B38" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G38" s="19"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B39" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G39" s="19"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B40" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B41" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" s="19" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B33" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B37" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F37" t="s">
-        <v>231</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="G38" s="12"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B39" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="G39" s="12"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B40" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="F41" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="G40" s="12" t="s">
+      <c r="G41" s="19" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B41" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="F41" t="s">
-        <v>235</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>238</v>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B42" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E42" s="19"/>
+      <c r="G42" s="19" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="B43" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F43" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -3552,47 +3717,47 @@
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -3615,139 +3780,139 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="13" t="s">
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13">
+        <v>0.121</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="E3" s="13">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="14">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="13">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13">
         <v>1</v>
       </c>
-      <c r="C3" s="14">
-        <v>0.121</v>
-      </c>
-      <c r="D3" s="14">
+      <c r="D4" s="13">
+        <v>0.498</v>
+      </c>
+      <c r="E4" s="13">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="13">
+        <v>3</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.627</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="13">
+        <v>4</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.153</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.157</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="13">
+        <v>5</v>
+      </c>
+      <c r="C7" s="13">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="13">
+        <v>6</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="13">
+        <v>7</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0.89</v>
+      </c>
+      <c r="D9" s="13">
         <v>0.46600000000000003</v>
       </c>
-      <c r="E3" s="14">
-        <v>0.70499999999999996</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="14">
-        <v>2</v>
-      </c>
-      <c r="C4" s="14">
-        <v>1</v>
-      </c>
-      <c r="D4" s="14">
-        <v>0.498</v>
-      </c>
-      <c r="E4" s="14">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="14">
-        <v>3</v>
-      </c>
-      <c r="C5" s="14">
-        <v>0.17199999999999999</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0.627</v>
-      </c>
-      <c r="E5" s="14">
-        <v>0.17199999999999999</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="14">
-        <v>4</v>
-      </c>
-      <c r="C6" s="14">
-        <v>0.83899999999999997</v>
-      </c>
-      <c r="D6" s="14">
-        <v>0.153</v>
-      </c>
-      <c r="E6" s="14">
-        <v>0.157</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="14">
-        <v>5</v>
-      </c>
-      <c r="C7" s="14">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="D7" s="14">
-        <v>0.40300000000000002</v>
-      </c>
-      <c r="E7" s="14">
-        <v>0.74099999999999999</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="14">
-        <v>6</v>
-      </c>
-      <c r="C8" s="14">
-        <v>0.54900000000000004</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0.33700000000000002</v>
-      </c>
-      <c r="E8" s="14">
-        <v>0.29399999999999998</v>
-      </c>
-      <c r="F8" s="14" t="s">
+      <c r="E9" s="13">
+        <v>0.76</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="14">
-        <v>7</v>
-      </c>
-      <c r="C9" s="14">
-        <v>0.89</v>
-      </c>
-      <c r="D9" s="14">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="E9" s="14">
-        <v>0.76</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
abstract out detect_decel_onset and detect_brake_jerk_end for reusability
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FEE350-00C1-0A4E-B1AE-0802C520B8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B744B7-CCD8-9A48-B042-E400A62E3487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="20400" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="1940" windowWidth="34200" windowHeight="20400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="297">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -801,18 +801,6 @@
   </si>
   <si>
     <t>brakeAccelMin</t>
-  </si>
-  <si>
-    <t>JERK_NEG_THD</t>
-  </si>
-  <si>
-    <t>JERK_POS_THD</t>
-  </si>
-  <si>
-    <t>Negative jerk threshold</t>
-  </si>
-  <si>
-    <t>Positive jerk threshold</t>
   </si>
   <si>
     <t>BRAKEJERK_MIN_SPEED</t>
@@ -923,6 +911,30 @@
   </si>
   <si>
     <t>end time of brake jerk</t>
+  </si>
+  <si>
+    <t>BRAKEJERK_JERK_NEG_THD</t>
+  </si>
+  <si>
+    <t>BRAKEJERK_JERK_POS_THD</t>
+  </si>
+  <si>
+    <t>AEB_JERK_NEG_THD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative jerk threshold to detect the start of AEB intervention </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative jerk threshold to detect the start of BrakeJerk intervention </t>
+  </si>
+  <si>
+    <t>Positive jerk threshold to detect the end of BrakeJerk intervention</t>
+  </si>
+  <si>
+    <t>LATENCY_WINDOW_SAMPLES</t>
+  </si>
+  <si>
+    <t>Sample window after AEB start for latency detection</t>
   </si>
 </sst>
 </file>
@@ -1591,7 +1603,7 @@
         <v>61</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>187</v>
@@ -1683,13 +1695,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D21" t="s">
         <v>187</v>
@@ -1700,10 +1712,10 @@
         <v>28</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D22" t="s">
         <v>187</v>
@@ -1778,15 +1790,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="4" width="8.83203125" customWidth="1"/>
     <col min="5" max="5" width="66.5" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" customWidth="1"/>
@@ -1848,7 +1860,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -1868,7 +1880,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2025,50 +2037,47 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>246</v>
+        <v>291</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>-30</v>
       </c>
       <c r="C13" t="s">
         <v>187</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>235</v>
       </c>
       <c r="E13" t="s">
-        <v>198</v>
+        <v>292</v>
       </c>
       <c r="F13" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>247</v>
+        <v>295</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>187</v>
-      </c>
-      <c r="D14" t="s">
-        <v>87</v>
+        <v>197</v>
       </c>
       <c r="E14" t="s">
-        <v>199</v>
+        <v>296</v>
       </c>
       <c r="F14" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
         <v>187</v>
@@ -2077,47 +2086,47 @@
         <v>87</v>
       </c>
       <c r="E15" t="s">
-        <v>245</v>
+        <v>198</v>
       </c>
       <c r="F15" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B16">
-        <v>-20</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
         <v>187</v>
       </c>
       <c r="D16" t="s">
-        <v>235</v>
+        <v>87</v>
       </c>
       <c r="E16" t="s">
-        <v>256</v>
+        <v>199</v>
       </c>
       <c r="F16" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="B17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
         <v>187</v>
       </c>
       <c r="D17" t="s">
-        <v>235</v>
+        <v>87</v>
       </c>
       <c r="E17" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="F17" t="s">
         <v>243</v>
@@ -2125,19 +2134,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>258</v>
+        <v>289</v>
       </c>
       <c r="B18">
-        <v>30</v>
+        <v>-20</v>
       </c>
       <c r="C18" t="s">
         <v>187</v>
       </c>
       <c r="D18" t="s">
-        <v>109</v>
+        <v>235</v>
       </c>
       <c r="E18" t="s">
-        <v>260</v>
+        <v>293</v>
       </c>
       <c r="F18" t="s">
         <v>243</v>
@@ -2145,19 +2154,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>259</v>
+        <v>290</v>
       </c>
       <c r="B19">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
         <v>187</v>
       </c>
       <c r="D19" t="s">
-        <v>109</v>
+        <v>235</v>
       </c>
       <c r="E19" t="s">
-        <v>261</v>
+        <v>294</v>
       </c>
       <c r="F19" t="s">
         <v>243</v>
@@ -2165,42 +2174,82 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
         <v>187</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="E20" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="F20" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>130</v>
       </c>
       <c r="C21" t="s">
         <v>187</v>
       </c>
       <c r="D21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" t="s">
+        <v>257</v>
+      </c>
+      <c r="F21" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>258</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>187</v>
+      </c>
+      <c r="D22" t="s">
         <v>87</v>
       </c>
-      <c r="E21" t="s">
-        <v>265</v>
-      </c>
-      <c r="F21" t="s">
-        <v>266</v>
+      <c r="E22" t="s">
+        <v>260</v>
+      </c>
+      <c r="F22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>259</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" t="s">
+        <v>261</v>
+      </c>
+      <c r="F23" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2271,7 +2320,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>37</v>
@@ -2766,7 +2815,7 @@
         <v>229</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>231</v>
@@ -2787,7 +2836,7 @@
         <v>17</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="J15" s="15" t="s">
         <v>24</v>
@@ -2804,7 +2853,7 @@
         <v>229</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>252</v>
@@ -2816,7 +2865,7 @@
         <v>80</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G16" s="15" t="b">
         <v>1</v>
@@ -2825,7 +2874,7 @@
         <v>17</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="J16" s="15" t="s">
         <v>24</v>
@@ -2842,7 +2891,7 @@
         <v>229</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>253</v>
@@ -2863,7 +2912,7 @@
         <v>17</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="J17" s="15" t="s">
         <v>24</v>
@@ -2880,10 +2929,10 @@
         <v>229</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D18" s="16">
         <v>0</v>
@@ -2892,7 +2941,7 @@
         <v>4</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="G18" s="15" t="b">
         <v>1</v>
@@ -2901,7 +2950,7 @@
         <v>17</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="J18" s="15" t="s">
         <v>24</v>
@@ -2925,8 +2974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE39B99-0AFB-8547-83BF-D855CC6E3BB3}">
   <dimension ref="B1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
@@ -3615,7 +3664,7 @@
         <v>87</v>
       </c>
       <c r="G38" s="19" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
@@ -3632,7 +3681,7 @@
         <v>87</v>
       </c>
       <c r="G39" s="19" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
@@ -3680,14 +3729,14 @@
         <v>229</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D42" s="19" t="s">
         <v>197</v>
       </c>
       <c r="E42" s="19"/>
       <c r="G42" s="19" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="96" x14ac:dyDescent="0.2">
@@ -3695,7 +3744,7 @@
         <v>229</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D43" s="19" t="s">
         <v>108</v>
@@ -3704,10 +3753,10 @@
         <v>87</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor scatter_plotter from a function into a class
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2432F9B-B937-694E-ABAB-7385906576FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C291C589-E408-0142-A46F-783128D814C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1940" windowWidth="34200" windowHeight="20400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="740" windowWidth="34200" windowHeight="20400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -1041,7 +1041,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1070,9 +1070,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1795,7 +1793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -2269,8 +2267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24310F59-1486-4F41-B3B7-AB25CE8F592D}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2817,154 +2815,154 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="2" t="s">
         <v>265</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D15" s="16">
-        <v>0</v>
-      </c>
-      <c r="E15" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="F15" s="15" t="s">
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="15" t="b">
+      <c r="G15" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="J15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15" s="15" t="b">
+      <c r="K15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="D16" s="16">
-        <v>0</v>
-      </c>
-      <c r="E16" s="16">
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
         <v>80</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="G16" s="15" t="b">
+      <c r="G16" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="H16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="J16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16" s="15" t="b">
+      <c r="K16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="3">
         <v>-6</v>
       </c>
-      <c r="E17" s="16">
-        <v>0</v>
-      </c>
-      <c r="F17" s="15" t="s">
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G17" s="15" t="b">
+      <c r="G17" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="H17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="I17" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="J17" s="15" t="s">
+      <c r="J17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L17" s="15" t="b">
+      <c r="K17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="D18" s="16">
-        <v>0</v>
-      </c>
-      <c r="E18" s="16">
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
         <v>4</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="G18" s="15" t="b">
+      <c r="G18" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="H18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="I18" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="J18" s="15" t="s">
+      <c r="J18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L18" s="15" t="b">
+      <c r="K18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2987,781 +2985,781 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="17" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.1640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" style="20" customWidth="1"/>
-    <col min="7" max="7" width="45.1640625" style="20" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="20"/>
+    <col min="1" max="1" width="2.83203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="17" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="18" customWidth="1"/>
+    <col min="7" max="7" width="45.1640625" style="18" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="2:7" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="15" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19" t="s">
+      <c r="F5" s="17"/>
+      <c r="G5" s="17" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6" s="19" t="s">
+      <c r="B6" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="17" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C8" s="19" t="s">
+      <c r="B8" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19" t="s">
+      <c r="F8" s="17"/>
+      <c r="G8" s="17" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19" t="s">
+      <c r="F9" s="17"/>
+      <c r="G9" s="17" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C10" s="19" t="s">
+      <c r="B10" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="19" t="s">
+      <c r="B11" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19" t="s">
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" s="19" t="s">
+      <c r="B12" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19" t="s">
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C13" s="19" t="s">
+      <c r="B13" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19" t="s">
+      <c r="F13" s="17"/>
+      <c r="G13" s="17" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C14" s="19" t="s">
+      <c r="B14" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19" t="s">
+      <c r="F14" s="17"/>
+      <c r="G14" s="17" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C15" s="19" t="s">
+      <c r="B15" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19" t="s">
+      <c r="F15" s="17"/>
+      <c r="G15" s="17" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C16" s="19" t="s">
+      <c r="B16" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19" t="s">
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C17" s="19" t="s">
+      <c r="B17" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19" t="s">
+      <c r="F17" s="17"/>
+      <c r="G17" s="17" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C18" s="19" t="s">
+      <c r="B18" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19" t="s">
+      <c r="F18" s="17"/>
+      <c r="G18" s="17" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C19" s="19" t="s">
+      <c r="B19" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="17" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C20" s="19" t="s">
+      <c r="B20" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C21" s="19" t="s">
+      <c r="B21" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19" t="s">
+      <c r="F21" s="17"/>
+      <c r="G21" s="17" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C22" s="19" t="s">
+      <c r="B22" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="F22" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="17" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C23" s="19" t="s">
+      <c r="B23" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19" t="s">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C24" s="19" t="s">
+      <c r="B24" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19" t="s">
+      <c r="F24" s="17"/>
+      <c r="G24" s="17" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25" s="19" t="s">
+      <c r="B25" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="17" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C26" s="19" t="s">
+      <c r="B26" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19" t="s">
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C27" s="19" t="s">
+      <c r="B27" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19" t="s">
+      <c r="F27" s="17"/>
+      <c r="G27" s="17" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C28" s="19" t="s">
+      <c r="B28" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="G28" s="19" t="s">
+      <c r="G28" s="17" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C29" s="19" t="s">
+      <c r="B29" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19" t="s">
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C30" s="19" t="s">
+      <c r="B30" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="G30" s="19" t="s">
+      <c r="G30" s="17" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C31" s="19" t="s">
+      <c r="B31" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="G31" s="19" t="s">
+      <c r="G31" s="17" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C32" s="19" t="s">
+      <c r="B32" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19" t="s">
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B33" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C33" s="19" t="s">
+      <c r="B33" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19" t="s">
+      <c r="F33" s="17"/>
+      <c r="G33" s="17" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C34" s="19" t="s">
+      <c r="B34" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19" t="s">
+      <c r="F34" s="17"/>
+      <c r="G34" s="17" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C35" s="19" t="s">
+      <c r="B35" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19" t="s">
+      <c r="F35" s="17"/>
+      <c r="G35" s="17" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C36" s="19" t="s">
+      <c r="B36" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19" t="s">
+      <c r="F36" s="17"/>
+      <c r="G36" s="17" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="F37" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="G37" s="19" t="s">
+      <c r="G37" s="17" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="G38" s="19" t="s">
+      <c r="G38" s="17" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D39" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="G39" s="19" t="s">
+      <c r="G39" s="17" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C40" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="G40" s="19" t="s">
+      <c r="G40" s="17" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="D41" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="F41" s="20" t="s">
+      <c r="F41" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="G41" s="19" t="s">
+      <c r="G41" s="17" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D42" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="E42" s="19"/>
-      <c r="G42" s="19" t="s">
+      <c r="E42" s="17"/>
+      <c r="G42" s="17" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="96" x14ac:dyDescent="0.2">
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E43" s="19" t="s">
+      <c r="E43" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F43" s="21" t="s">
+      <c r="F43" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="G43" s="19" t="s">
+      <c r="G43" s="17" t="s">
         <v>279</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add avareage calculation feature
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C291C589-E408-0142-A46F-783128D814C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC02DC2-2189-1849-B244-AAE8B1F0C187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-80" yWindow="740" windowWidth="34200" windowHeight="20400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2268,7 +2268,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2374,7 +2374,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>68</v>
@@ -2979,7 +2979,7 @@
   <dimension ref="B1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remove parameter start_decel_aeb and end_decel_aeb
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC02DC2-2189-1849-B244-AAE8B1F0C187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B77373-FDB6-BC4B-B0C2-9F6D0954434F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="740" windowWidth="34200" windowHeight="20400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="700" windowWidth="34200" windowHeight="20360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="294">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -681,18 +681,6 @@
   </si>
   <si>
     <t>Class</t>
-  </si>
-  <si>
-    <t>START_DECEL_DELTA</t>
-  </si>
-  <si>
-    <t>threshold for large negative change (event start)</t>
-  </si>
-  <si>
-    <t>END_DECEL_DELTA</t>
-  </si>
-  <si>
-    <t># threshold for positive change (event end)</t>
   </si>
   <si>
     <t>InputHandler</t>
@@ -1604,7 +1592,7 @@
         <v>61</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>187</v>
@@ -1621,7 +1609,7 @@
         <v>63</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1635,7 +1623,7 @@
         <v>65</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1649,60 +1637,60 @@
         <v>181</v>
       </c>
       <c r="D17" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C18" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="D18" t="s">
         <v>222</v>
-      </c>
-      <c r="D18" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D19" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>224</v>
-      </c>
       <c r="C20" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D20" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D21" t="s">
         <v>187</v>
@@ -1713,10 +1701,10 @@
         <v>28</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D22" t="s">
         <v>187</v>
@@ -1791,10 +1779,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1827,7 +1815,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B2">
         <v>0.01</v>
@@ -1842,12 +1830,12 @@
         <v>200</v>
       </c>
       <c r="F2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -1856,15 +1844,15 @@
         <v>197</v>
       </c>
       <c r="E3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -1879,12 +1867,12 @@
         <v>198</v>
       </c>
       <c r="F4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1899,35 +1887,32 @@
         <v>199</v>
       </c>
       <c r="F5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>214</v>
+        <v>188</v>
       </c>
       <c r="B6">
-        <v>-30</v>
+        <v>300</v>
       </c>
       <c r="C6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D6" t="s">
-        <v>156</v>
+        <v>197</v>
       </c>
       <c r="E6" t="s">
-        <v>215</v>
+        <v>293</v>
       </c>
       <c r="F6" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>189</v>
       </c>
       <c r="B7">
-        <v>29</v>
+        <v>-6</v>
       </c>
       <c r="C7" t="s">
         <v>187</v>
@@ -1936,35 +1921,38 @@
         <v>156</v>
       </c>
       <c r="E7" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="F7" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B8">
-        <v>300</v>
+        <v>-15</v>
       </c>
       <c r="C8" t="s">
-        <v>197</v>
+        <v>187</v>
+      </c>
+      <c r="D8" t="s">
+        <v>156</v>
       </c>
       <c r="E8" t="s">
-        <v>297</v>
+        <v>194</v>
       </c>
       <c r="F8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B9">
-        <v>-6</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="C9" t="s">
         <v>187</v>
@@ -1973,18 +1961,18 @@
         <v>156</v>
       </c>
       <c r="E9" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F9" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B10">
-        <v>-15</v>
+        <v>0.2</v>
       </c>
       <c r="C10" t="s">
         <v>187</v>
@@ -1993,95 +1981,95 @@
         <v>156</v>
       </c>
       <c r="E10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F10" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>286</v>
       </c>
       <c r="B11">
-        <v>-4.9000000000000004</v>
+        <v>-30</v>
       </c>
       <c r="C11" t="s">
         <v>187</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
+        <v>230</v>
       </c>
       <c r="E11" t="s">
-        <v>195</v>
+        <v>287</v>
       </c>
       <c r="F11" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>192</v>
+        <v>290</v>
       </c>
       <c r="B12">
-        <v>0.2</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>187</v>
-      </c>
-      <c r="D12" t="s">
-        <v>156</v>
+        <v>197</v>
       </c>
       <c r="E12" t="s">
-        <v>196</v>
+        <v>291</v>
       </c>
       <c r="F12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>290</v>
+        <v>241</v>
       </c>
       <c r="B13">
-        <v>-30</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
         <v>187</v>
       </c>
       <c r="D13" t="s">
-        <v>234</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
-        <v>291</v>
+        <v>198</v>
       </c>
       <c r="F13" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>294</v>
+        <v>242</v>
       </c>
       <c r="B14">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>197</v>
+        <v>187</v>
+      </c>
+      <c r="D14" t="s">
+        <v>87</v>
       </c>
       <c r="E14" t="s">
-        <v>295</v>
+        <v>199</v>
       </c>
       <c r="F14" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
         <v>187</v>
@@ -2090,90 +2078,90 @@
         <v>87</v>
       </c>
       <c r="E15" t="s">
-        <v>198</v>
+        <v>240</v>
       </c>
       <c r="F15" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>246</v>
+        <v>284</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>-20</v>
       </c>
       <c r="C16" t="s">
         <v>187</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>230</v>
       </c>
       <c r="E16" t="s">
-        <v>199</v>
+        <v>288</v>
       </c>
       <c r="F16" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>243</v>
+        <v>285</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>187</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>230</v>
       </c>
       <c r="E17" t="s">
-        <v>244</v>
+        <v>289</v>
       </c>
       <c r="F17" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>288</v>
+        <v>249</v>
       </c>
       <c r="B18">
-        <v>-20</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>187</v>
       </c>
       <c r="D18" t="s">
-        <v>234</v>
+        <v>109</v>
       </c>
       <c r="E18" t="s">
-        <v>292</v>
+        <v>251</v>
       </c>
       <c r="F18" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>289</v>
+        <v>250</v>
       </c>
       <c r="B19">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C19" t="s">
         <v>187</v>
       </c>
       <c r="D19" t="s">
-        <v>234</v>
+        <v>109</v>
       </c>
       <c r="E19" t="s">
-        <v>293</v>
+        <v>252</v>
       </c>
       <c r="F19" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2181,19 +2169,19 @@
         <v>253</v>
       </c>
       <c r="B20">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
         <v>187</v>
       </c>
       <c r="D20" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="E20" t="s">
         <v>255</v>
       </c>
       <c r="F20" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2201,59 +2189,19 @@
         <v>254</v>
       </c>
       <c r="B21">
-        <v>130</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
         <v>187</v>
       </c>
       <c r="D21" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s">
         <v>256</v>
       </c>
       <c r="F21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
         <v>257</v>
-      </c>
-      <c r="B22">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
-        <v>187</v>
-      </c>
-      <c r="D22" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" t="s">
-        <v>259</v>
-      </c>
-      <c r="F22" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>258</v>
-      </c>
-      <c r="B23">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D23" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" t="s">
-        <v>260</v>
-      </c>
-      <c r="F23" t="s">
-        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -2267,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24310F59-1486-4F41-B3B7-AB25CE8F592D}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2324,7 +2272,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>37</v>
@@ -2816,13 +2764,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D15" s="3">
         <v>0</v>
@@ -2840,7 +2788,7 @@
         <v>17</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>24</v>
@@ -2854,13 +2802,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D16" s="3">
         <v>0</v>
@@ -2869,7 +2817,7 @@
         <v>80</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G16" s="2" t="b">
         <v>1</v>
@@ -2878,7 +2826,7 @@
         <v>17</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>24</v>
@@ -2892,13 +2840,13 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D17" s="3">
         <v>-6</v>
@@ -2916,7 +2864,7 @@
         <v>17</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>24</v>
@@ -2930,13 +2878,13 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D18" s="3">
         <v>0</v>
@@ -2945,7 +2893,7 @@
         <v>4</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G18" s="2" t="b">
         <v>1</v>
@@ -2954,7 +2902,7 @@
         <v>17</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>24</v>
@@ -3017,23 +2965,23 @@
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="17" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
       <c r="G2" s="17" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="17" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>107</v>
@@ -3051,7 +2999,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="17" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>29</v>
@@ -3636,10 +3584,10 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" s="17" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D37" s="17" t="s">
         <v>108</v>
@@ -3648,18 +3596,18 @@
         <v>87</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" s="17" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D38" s="17" t="s">
         <v>108</v>
@@ -3668,15 +3616,15 @@
         <v>87</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="17" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D39" s="17" t="s">
         <v>108</v>
@@ -3685,35 +3633,35 @@
         <v>87</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" s="17" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D40" s="17" t="s">
         <v>108</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" s="17" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D41" s="17" t="s">
         <v>108</v>
@@ -3722,33 +3670,33 @@
         <v>156</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B42" s="17" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D42" s="17" t="s">
         <v>197</v>
       </c>
       <c r="E42" s="17"/>
       <c r="G42" s="17" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="96" x14ac:dyDescent="0.2">
       <c r="B43" s="17" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D43" s="17" t="s">
         <v>108</v>
@@ -3757,10 +3705,10 @@
         <v>87</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
communication latency calculation added
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B77373-FDB6-BC4B-B0C2-9F6D0954434F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08F153F-E8C1-FA43-A9B1-909C4D6FC3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="700" windowWidth="34200" windowHeight="20360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="20360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="299">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -926,6 +926,21 @@
   </si>
   <si>
     <t>window of samples (~3s at 0.01s rate) prior to AEB intervention, used for precondition evaluation</t>
+  </si>
+  <si>
+    <t>PB_DURATION</t>
+  </si>
+  <si>
+    <t>Minimum duration (s) that partial braking must persist before transitioning to full braking.</t>
+  </si>
+  <si>
+    <t>commLatency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communication latency </t>
+  </si>
+  <si>
+    <t>Communication Latency</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1044,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1074,6 +1089,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1779,10 +1796,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1949,19 +1966,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>294</v>
       </c>
       <c r="B9">
-        <v>-4.9000000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="C9" t="s">
         <v>187</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>87</v>
       </c>
       <c r="E9" t="s">
-        <v>195</v>
+        <v>295</v>
       </c>
       <c r="F9" t="s">
         <v>237</v>
@@ -1969,10 +1986,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B10">
-        <v>0.2</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="C10" t="s">
         <v>187</v>
@@ -1981,7 +1998,7 @@
         <v>156</v>
       </c>
       <c r="E10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F10" t="s">
         <v>237</v>
@@ -1989,19 +2006,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>286</v>
+        <v>192</v>
       </c>
       <c r="B11">
-        <v>-30</v>
+        <v>0.2</v>
       </c>
       <c r="C11" t="s">
         <v>187</v>
       </c>
       <c r="D11" t="s">
-        <v>230</v>
+        <v>156</v>
       </c>
       <c r="E11" t="s">
-        <v>287</v>
+        <v>196</v>
       </c>
       <c r="F11" t="s">
         <v>237</v>
@@ -2009,16 +2026,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B12">
-        <v>30</v>
+        <v>-25</v>
       </c>
       <c r="C12" t="s">
-        <v>197</v>
+        <v>187</v>
+      </c>
+      <c r="D12" t="s">
+        <v>230</v>
       </c>
       <c r="E12" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F12" t="s">
         <v>237</v>
@@ -2026,30 +2046,27 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>241</v>
+        <v>290</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>187</v>
-      </c>
-      <c r="D13" t="s">
-        <v>87</v>
+        <v>197</v>
       </c>
       <c r="E13" t="s">
-        <v>198</v>
+        <v>291</v>
       </c>
       <c r="F13" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
         <v>187</v>
@@ -2058,7 +2075,7 @@
         <v>87</v>
       </c>
       <c r="E14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F14" t="s">
         <v>243</v>
@@ -2066,10 +2083,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
         <v>187</v>
@@ -2078,27 +2095,27 @@
         <v>87</v>
       </c>
       <c r="E15" t="s">
-        <v>240</v>
+        <v>199</v>
       </c>
       <c r="F15" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>284</v>
+        <v>239</v>
       </c>
       <c r="B16">
-        <v>-20</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
         <v>187</v>
       </c>
       <c r="D16" t="s">
-        <v>230</v>
+        <v>87</v>
       </c>
       <c r="E16" t="s">
-        <v>288</v>
+        <v>240</v>
       </c>
       <c r="F16" t="s">
         <v>238</v>
@@ -2106,10 +2123,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B17">
-        <v>20</v>
+        <v>-20</v>
       </c>
       <c r="C17" t="s">
         <v>187</v>
@@ -2118,7 +2135,7 @@
         <v>230</v>
       </c>
       <c r="E17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F17" t="s">
         <v>238</v>
@@ -2126,19 +2143,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>249</v>
+        <v>285</v>
       </c>
       <c r="B18">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
         <v>187</v>
       </c>
       <c r="D18" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
       <c r="E18" t="s">
-        <v>251</v>
+        <v>289</v>
       </c>
       <c r="F18" t="s">
         <v>238</v>
@@ -2146,10 +2163,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B19">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
         <v>187</v>
@@ -2158,7 +2175,7 @@
         <v>109</v>
       </c>
       <c r="E19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F19" t="s">
         <v>238</v>
@@ -2166,30 +2183,30 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>130</v>
       </c>
       <c r="C20" t="s">
         <v>187</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="E20" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F20" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>187</v>
@@ -2198,9 +2215,29 @@
         <v>87</v>
       </c>
       <c r="E21" t="s">
+        <v>255</v>
+      </c>
+      <c r="F21" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>254</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>187</v>
+      </c>
+      <c r="D22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" t="s">
         <v>256</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" t="s">
         <v>257</v>
       </c>
     </row>
@@ -2215,8 +2252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24310F59-1486-4F41-B3B7-AB25CE8F592D}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2915,7 +2952,42 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
+      <c r="A19" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="D19" s="21">
+        <v>0</v>
+      </c>
+      <c r="E19" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L19" s="20" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2924,11 +2996,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE39B99-0AFB-8547-83BF-D855CC6E3BB3}">
-  <dimension ref="B1:G43"/>
+  <dimension ref="B1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3709,6 +3781,23 @@
       </c>
       <c r="G43" s="17" t="s">
         <v>275</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B44" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
communication latency jerk thd bug fixed
</commit_message>
<xml_diff>
--- a/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_kpi_extractor/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08F153F-E8C1-FA43-A9B1-909C4D6FC3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CFD35C-2AF9-344C-9490-B8817B0DFB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="20360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="20360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="301">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -941,6 +941,12 @@
   </si>
   <si>
     <t>Communication Latency</t>
+  </si>
+  <si>
+    <t>Negative jerk threshold to detect the start of full braking</t>
+  </si>
+  <si>
+    <t>FB_JERK_NEG_THD</t>
   </si>
 </sst>
 </file>
@@ -1796,10 +1802,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2046,16 +2052,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="B13">
-        <v>30</v>
+        <v>-20</v>
       </c>
       <c r="C13" t="s">
-        <v>197</v>
+        <v>187</v>
+      </c>
+      <c r="D13" t="s">
+        <v>230</v>
       </c>
       <c r="E13" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="F13" t="s">
         <v>237</v>
@@ -2063,30 +2072,27 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>241</v>
+        <v>290</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>187</v>
-      </c>
-      <c r="D14" t="s">
-        <v>87</v>
+        <v>197</v>
       </c>
       <c r="E14" t="s">
-        <v>198</v>
+        <v>291</v>
       </c>
       <c r="F14" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
         <v>187</v>
@@ -2095,7 +2101,7 @@
         <v>87</v>
       </c>
       <c r="E15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F15" t="s">
         <v>243</v>
@@ -2103,10 +2109,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
         <v>187</v>
@@ -2115,27 +2121,27 @@
         <v>87</v>
       </c>
       <c r="E16" t="s">
-        <v>240</v>
+        <v>199</v>
       </c>
       <c r="F16" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>284</v>
+        <v>239</v>
       </c>
       <c r="B17">
-        <v>-20</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
         <v>187</v>
       </c>
       <c r="D17" t="s">
-        <v>230</v>
+        <v>87</v>
       </c>
       <c r="E17" t="s">
-        <v>288</v>
+        <v>240</v>
       </c>
       <c r="F17" t="s">
         <v>238</v>
@@ -2143,10 +2149,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B18">
-        <v>20</v>
+        <v>-20</v>
       </c>
       <c r="C18" t="s">
         <v>187</v>
@@ -2155,7 +2161,7 @@
         <v>230</v>
       </c>
       <c r="E18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F18" t="s">
         <v>238</v>
@@ -2163,19 +2169,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>249</v>
+        <v>285</v>
       </c>
       <c r="B19">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
         <v>187</v>
       </c>
       <c r="D19" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
       <c r="E19" t="s">
-        <v>251</v>
+        <v>289</v>
       </c>
       <c r="F19" t="s">
         <v>238</v>
@@ -2183,10 +2189,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B20">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
         <v>187</v>
@@ -2195,7 +2201,7 @@
         <v>109</v>
       </c>
       <c r="E20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F20" t="s">
         <v>238</v>
@@ -2203,30 +2209,30 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>130</v>
       </c>
       <c r="C21" t="s">
         <v>187</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="E21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F21" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
         <v>187</v>
@@ -2235,9 +2241,29 @@
         <v>87</v>
       </c>
       <c r="E22" t="s">
+        <v>255</v>
+      </c>
+      <c r="F22" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>254</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" t="s">
         <v>256</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
         <v>257</v>
       </c>
     </row>
@@ -2252,7 +2278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24310F59-1486-4F41-B3B7-AB25CE8F592D}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>

</xml_diff>